<commit_message>
Alteração na automação realizando o request e criando o body request apartir de uma planilha
</commit_message>
<xml_diff>
--- a/xml/massa_xml.xlsx
+++ b/xml/massa_xml.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\QA_ALLIANZ\xml\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7F8DAE-9BC7-4C24-BADE-213E0A1B0A04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70995FD7-AE46-4F47-81DA-93D781899F9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{53E9DAE5-326D-4ECB-A2E7-4BBDF0D5EA43}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>usuario</t>
   </si>
@@ -218,42 +219,23 @@
     <t>270</t>
   </si>
   <si>
-    <t>BA262881</t>
-  </si>
-  <si>
-    <t>2019-03-12</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>1985-03-22</t>
-  </si>
-  <si>
-    <t>9BRBL3HE6K0175836</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>PEA1636</t>
-  </si>
-  <si>
-    <t>201</t>
-  </si>
-  <si>
-    <t>262</t>
-  </si>
-  <si>
-    <t>teste</t>
+    <t>0617120</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -281,9 +263,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225BDF44-9FA6-4B52-B8E5-3ADE615B34D2}">
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="AN20" sqref="AN20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,8 +697,8 @@
       <c r="B2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="1">
-        <v>617120</v>
+      <c r="C2" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
@@ -805,107 +788,6 @@
         <v>60</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="1">
-        <v>617121</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="1">
-        <v>31</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG3" s="1" t="s">
         <v>61</v>
       </c>
     </row>
@@ -913,4 +795,22 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{918C16A6-E27E-4D2C-9032-CCE09DFC5198}">
+  <dimension ref="C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>